<commit_message>
adding sprint 1 files
</commit_message>
<xml_diff>
--- a/TeamAchalAkankshaSaloniSravanthiReport.xlsx
+++ b/TeamAchalAkankshaSaloniSravanthiReport.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SEM 3\Agile\project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="208">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -157,10 +157,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Review Results</t>
   </si>
   <si>
@@ -176,15 +172,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
   <si>
@@ -548,9 +535,6 @@
     <t>US42</t>
   </si>
   <si>
-    <t>Coding</t>
-  </si>
-  <si>
     <t>Dates before current date</t>
   </si>
   <si>
@@ -672,6 +656,39 @@
   </si>
   <si>
     <t>achalav</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>SSK</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AV</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicating with the team members </t>
+  </si>
+  <si>
+    <t>Updating the source code on regular basis</t>
+  </si>
+  <si>
+    <t>Integration at the last moment</t>
+  </si>
+  <si>
+    <t>coding</t>
   </si>
 </sst>
 </file>
@@ -962,10 +979,10 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>41065</c:v>
+                  <c:v>41535</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41078</c:v>
+                  <c:v>41549</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41092</c:v>
@@ -986,19 +1003,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,8 +1104,14 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>41535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41549</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1109,6 +1123,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1133,24 +1150,23 @@
         <c:axId val="-467596544"/>
         <c:axId val="-467594224"/>
       </c:lineChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="-467596544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-467594224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="1"/>
-      </c:catAx>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="-467594224"/>
         <c:scaling>
@@ -1223,15 +1239,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>469053</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25401</xdr:rowOff>
+      <xdr:colOff>342053</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>40641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>948266</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>160867</xdr:rowOff>
+      <xdr:colOff>821266</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>13547</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1246,8 +1262,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1425786" y="533401"/>
-          <a:ext cx="1317413" cy="643466"/>
+          <a:off x="1251373" y="1178561"/>
+          <a:ext cx="1271693" cy="623146"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -2025,83 +2041,83 @@
         <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
         <v>181</v>
       </c>
-      <c r="B3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
       <c r="D3" s="20" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" t="s">
         <v>192</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="E5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2141,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2159,16 +2175,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2176,13 +2192,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2190,13 +2209,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2204,13 +2226,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2218,16 +2243,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2235,13 +2260,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="E7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2249,222 +2277,273 @@
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" t="s">
-        <v>182</v>
-      </c>
-      <c r="E8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="17" t="s">
+      <c r="C12" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+      <c r="C13" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="17" t="s">
+      <c r="C14" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="17" t="s">
+      <c r="C15" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C16" s="17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
+      <c r="D16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C17" s="17" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="17" t="s">
+      <c r="D17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C18" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="17" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="17" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C21" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="17" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="17" t="s">
+      <c r="C23" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="17" t="s">
+      <c r="C24" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="17" t="s">
+      <c r="C25" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="17" t="s">
+      <c r="C26" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="17" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="17" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="17" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="17" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C31" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B28" s="17" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B32" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2478,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2494,37 +2573,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -2547,13 +2626,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B15" s="12">
-        <v>41065</v>
+        <v>41535</v>
       </c>
       <c r="C15" s="13">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E15" s="13">
         <v>0</v>
@@ -2563,103 +2642,64 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B16" s="12">
-        <v>41078</v>
+        <v>41549</v>
       </c>
       <c r="C16" s="13">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E16" s="13">
-        <v>250</v>
+        <v>1054</v>
       </c>
       <c r="F16" s="13">
-        <v>120</v>
+        <v>220</v>
       </c>
       <c r="G16" s="9">
         <f>(E16-E15)/F16*60</f>
-        <v>125.00000000000001</v>
+        <v>287.45454545454544</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B17" s="12">
         <v>41092</v>
       </c>
-      <c r="C17" s="13">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <f t="shared" ref="D17:D19" si="0">C16-C17</f>
-        <v>6</v>
-      </c>
-      <c r="E17" s="13">
-        <v>480</v>
-      </c>
-      <c r="F17" s="14">
-        <v>135</v>
-      </c>
-      <c r="G17" s="9">
-        <f t="shared" ref="G17:G19" si="1">(E17-E16)/F17*60</f>
-        <v>102.22222222222223</v>
-      </c>
+      <c r="C17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B18" s="12">
         <v>41106</v>
       </c>
-      <c r="C18" s="13">
-        <v>6</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E18" s="13">
-        <v>740</v>
-      </c>
-      <c r="F18" s="14">
-        <v>160</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="1"/>
-        <v>97.5</v>
-      </c>
+      <c r="C18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B19" s="12">
         <v>41120</v>
       </c>
-      <c r="C19" s="13">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E19" s="13">
-        <v>1100</v>
-      </c>
-      <c r="F19" s="14">
-        <v>145</v>
-      </c>
-      <c r="G19" s="9">
-        <f t="shared" si="1"/>
-        <v>148.9655172413793</v>
-      </c>
+      <c r="C19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2670,10 +2710,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2707,8 +2747,37 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>41535</v>
+      </c>
       <c r="B2">
         <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>41549</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>1054</v>
+      </c>
+      <c r="E3">
+        <v>220</v>
+      </c>
+      <c r="F3" s="9">
+        <v>287.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f>Burndown!C36</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2723,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2770,16 +2839,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -2787,114 +2856,222 @@
       <c r="F2">
         <v>180</v>
       </c>
+      <c r="G2">
+        <v>158</v>
+      </c>
+      <c r="H2">
+        <v>240</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3">
+        <v>120</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>148</v>
+      </c>
+      <c r="H3">
+        <v>180</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>73</v>
+      <c r="A4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>176</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="G4">
+        <v>88</v>
+      </c>
+      <c r="H4">
+        <v>120</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>180</v>
+      </c>
+      <c r="G5">
+        <v>115</v>
+      </c>
+      <c r="H5">
         <v>120</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>181</v>
+      <c r="I5" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="F6">
+        <v>60</v>
+      </c>
+      <c r="G6">
+        <v>124</v>
+      </c>
+      <c r="H6">
         <v>180</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>184</v>
+        <v>179</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>120</v>
+      </c>
+      <c r="G7">
+        <v>127</v>
+      </c>
+      <c r="H7">
+        <v>180</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8">
         <v>30</v>
-      </c>
-      <c r="E8">
-        <v>25</v>
       </c>
       <c r="F8">
         <v>120</v>
       </c>
+      <c r="G8">
+        <v>151</v>
+      </c>
+      <c r="H8">
+        <v>240</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="E9">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="F9">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>143</v>
+      </c>
+      <c r="H9">
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" t="s">
-        <v>182</v>
+      <c r="I9" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2903,27 +3080,27 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2935,10 +3112,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -2970,6 +3147,154 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8">
+        <v>80</v>
+      </c>
+      <c r="F8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3073,8 +3398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B33"/>
+    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -3087,475 +3412,475 @@
   <sheetData>
     <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>118</v>
+      <c r="A2" s="21" t="s">
+        <v>199</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>